<commit_message>
edited data with new changes
</commit_message>
<xml_diff>
--- a/Cleaned_Cagayan/Daily_Data.xlsx
+++ b/Cleaned_Cagayan/Daily_Data.xlsx
@@ -19,103 +19,103 @@
     <t>Water_Level</t>
   </si>
   <si>
-    <t>RG0_Diff</t>
+    <t>RG_Diff</t>
   </si>
   <si>
     <t>Timestamp</t>
   </si>
   <si>
-    <t>2021/10/1</t>
-  </si>
-  <si>
-    <t>2021/10/2</t>
-  </si>
-  <si>
-    <t>2021/10/3</t>
-  </si>
-  <si>
-    <t>2021/10/4</t>
-  </si>
-  <si>
-    <t>2021/10/5</t>
-  </si>
-  <si>
-    <t>2021/10/6</t>
-  </si>
-  <si>
-    <t>2021/10/7</t>
-  </si>
-  <si>
-    <t>2021/10/8</t>
-  </si>
-  <si>
-    <t>2021/10/9</t>
-  </si>
-  <si>
-    <t>2021/10/10</t>
-  </si>
-  <si>
-    <t>2021/10/11</t>
-  </si>
-  <si>
-    <t>2021/10/12</t>
-  </si>
-  <si>
-    <t>2021/10/13</t>
-  </si>
-  <si>
-    <t>2021/10/14</t>
-  </si>
-  <si>
-    <t>2021/10/15</t>
-  </si>
-  <si>
-    <t>2021/10/16</t>
-  </si>
-  <si>
-    <t>2021/10/17</t>
-  </si>
-  <si>
-    <t>2021/10/18</t>
-  </si>
-  <si>
-    <t>2021/10/19</t>
-  </si>
-  <si>
-    <t>2021/10/20</t>
-  </si>
-  <si>
-    <t>2021/10/21</t>
-  </si>
-  <si>
-    <t>2021/10/22</t>
-  </si>
-  <si>
-    <t>2021/10/23</t>
-  </si>
-  <si>
-    <t>2021/10/24</t>
-  </si>
-  <si>
-    <t>2021/10/25</t>
-  </si>
-  <si>
-    <t>2021/10/26</t>
-  </si>
-  <si>
-    <t>2021/10/27</t>
-  </si>
-  <si>
-    <t>2021/10/28</t>
-  </si>
-  <si>
-    <t>2021/10/29</t>
-  </si>
-  <si>
-    <t>2021/10/30</t>
-  </si>
-  <si>
-    <t>2021/10/31</t>
+    <t>2021/12/1</t>
+  </si>
+  <si>
+    <t>2021/12/2</t>
+  </si>
+  <si>
+    <t>2021/12/3</t>
+  </si>
+  <si>
+    <t>2021/12/4</t>
+  </si>
+  <si>
+    <t>2021/12/5</t>
+  </si>
+  <si>
+    <t>2021/12/6</t>
+  </si>
+  <si>
+    <t>2021/12/7</t>
+  </si>
+  <si>
+    <t>2021/12/8</t>
+  </si>
+  <si>
+    <t>2021/12/9</t>
+  </si>
+  <si>
+    <t>2021/12/10</t>
+  </si>
+  <si>
+    <t>2021/12/11</t>
+  </si>
+  <si>
+    <t>2021/12/12</t>
+  </si>
+  <si>
+    <t>2021/12/13</t>
+  </si>
+  <si>
+    <t>2021/12/14</t>
+  </si>
+  <si>
+    <t>2021/12/15</t>
+  </si>
+  <si>
+    <t>2021/12/16</t>
+  </si>
+  <si>
+    <t>2021/12/17</t>
+  </si>
+  <si>
+    <t>2021/12/18</t>
+  </si>
+  <si>
+    <t>2021/12/19</t>
+  </si>
+  <si>
+    <t>2021/12/20</t>
+  </si>
+  <si>
+    <t>2021/12/21</t>
+  </si>
+  <si>
+    <t>2021/12/22</t>
+  </si>
+  <si>
+    <t>2021/12/23</t>
+  </si>
+  <si>
+    <t>2021/12/24</t>
+  </si>
+  <si>
+    <t>2021/12/25</t>
+  </si>
+  <si>
+    <t>2021/12/26</t>
+  </si>
+  <si>
+    <t>2021/12/27</t>
+  </si>
+  <si>
+    <t>2021/12/28</t>
+  </si>
+  <si>
+    <t>2021/12/29</t>
+  </si>
+  <si>
+    <t>2021/12/30</t>
+  </si>
+  <si>
+    <t>2021/12/31</t>
   </si>
 </sst>
 </file>
@@ -495,10 +495,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>2.800815</v>
+        <v>1.606017</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2.84248</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -506,10 +506,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>3.01569</v>
+        <v>1.29442</v>
       </c>
       <c r="C3">
-        <v>29.60000000000002</v>
+        <v>5.26993</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -517,10 +517,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>2.514315</v>
+        <v>1.701893</v>
       </c>
       <c r="C4">
-        <v>3.200000000000045</v>
+        <v>12.51669</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -528,10 +528,10 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>2.25169</v>
+        <v>1.253330285714286</v>
       </c>
       <c r="C5">
-        <v>10.39999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -539,10 +539,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>2.227815</v>
+        <v>1.198544</v>
       </c>
       <c r="C6">
-        <v>10.39999999999998</v>
+        <v>0.02434</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -550,10 +550,10 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>2.227815</v>
+        <v>1.198544</v>
       </c>
       <c r="C7">
-        <v>7</v>
+        <v>0.01687</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -561,10 +561,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>2.227815</v>
+        <v>1.174575</v>
       </c>
       <c r="C8">
-        <v>0.2000000000000455</v>
+        <v>0.16428</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -572,10 +572,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>2.227815</v>
+        <v>1.126637</v>
       </c>
       <c r="C9">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -583,10 +583,10 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>2.227815</v>
+        <v>1.126637</v>
       </c>
       <c r="C10">
-        <v>4.600000000000023</v>
+        <v>3.33038</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -594,10 +594,10 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>2.227815</v>
+        <v>1.510141</v>
       </c>
       <c r="C11">
-        <v>3.399999999999999</v>
+        <v>2.90854</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -605,10 +605,10 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>2.227815</v>
+        <v>1.869676</v>
       </c>
       <c r="C12">
-        <v>0.8000000000000007</v>
+        <v>2.39</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -616,10 +616,10 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>2.227815</v>
+        <v>1.582048</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>5.99</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -627,10 +627,10 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>2.227815</v>
+        <v>1.917614</v>
       </c>
       <c r="C14">
-        <v>1.799999999999999</v>
+        <v>3.21371</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -638,10 +638,10 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>2.227815</v>
+        <v>1.7738</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>0.7083699999999999</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -649,10 +649,10 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>2.227815</v>
+        <v>1.246482</v>
       </c>
       <c r="C16">
-        <v>3.200000000000001</v>
+        <v>10.67993</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -660,10 +660,10 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>2.227815</v>
+        <v>2.041090666666666</v>
       </c>
       <c r="C17">
-        <v>0.1999999999999993</v>
+        <v>20.68171</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -671,10 +671,10 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>2.227815</v>
+        <v>2.396994</v>
       </c>
       <c r="C18">
-        <v>18.6</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -682,10 +682,10 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>2.227815</v>
+        <v>1.845707</v>
       </c>
       <c r="C19">
-        <v>0.1999999999999993</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -693,10 +693,10 @@
         <v>21</v>
       </c>
       <c r="B20">
-        <v>2.227815</v>
+        <v>1.582048</v>
       </c>
       <c r="C20">
-        <v>9.800000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -704,10 +704,10 @@
         <v>22</v>
       </c>
       <c r="B21">
-        <v>2.227815</v>
+        <v>1.414265</v>
       </c>
       <c r="C21">
-        <v>3.399999999999999</v>
+        <v>1.39796</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -715,10 +715,10 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>2.227815</v>
+        <v>1.318389</v>
       </c>
       <c r="C22">
-        <v>0.1999999999999957</v>
+        <v>1.05275</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -726,10 +726,10 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>2.227815</v>
+        <v>1.246482</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>0.25737</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -737,10 +737,10 @@
         <v>25</v>
       </c>
       <c r="B24">
-        <v>2.227815</v>
+        <v>1.198544</v>
       </c>
       <c r="C24">
-        <v>7.400000000000006</v>
+        <v>0.03491</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -748,10 +748,10 @@
         <v>26</v>
       </c>
       <c r="B25">
-        <v>2.227815</v>
+        <v>1.174575</v>
       </c>
       <c r="C25">
-        <v>0.1999999999999957</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -759,10 +759,10 @@
         <v>27</v>
       </c>
       <c r="B26">
-        <v>2.227815</v>
+        <v>1.342358</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>2.94</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -770,10 +770,10 @@
         <v>28</v>
       </c>
       <c r="B27">
-        <v>2.227815</v>
+        <v>1.318389</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -781,10 +781,10 @@
         <v>29</v>
       </c>
       <c r="B28">
-        <v>2.227815</v>
+        <v>1.342358</v>
       </c>
       <c r="C28">
-        <v>60.2</v>
+        <v>0.47368</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -792,10 +792,10 @@
         <v>30</v>
       </c>
       <c r="B29">
-        <v>2.227815</v>
+        <v>1.270451</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>2.13196</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -803,10 +803,10 @@
         <v>31</v>
       </c>
       <c r="B30">
-        <v>2.227815</v>
+        <v>1.078699</v>
       </c>
       <c r="C30">
-        <v>3.200000000000003</v>
+        <v>3.58021</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -814,10 +814,10 @@
         <v>32</v>
       </c>
       <c r="B31">
-        <v>2.227815</v>
+        <v>1.078699</v>
       </c>
       <c r="C31">
-        <v>2.799999999999997</v>
+        <v>0.0492</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -825,10 +825,10 @@
         <v>33</v>
       </c>
       <c r="B32">
-        <v>2.227815</v>
+        <v>1.174575</v>
       </c>
       <c r="C32">
-        <v>3.200000000000003</v>
+        <v>2.50025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>